<commit_message>
added df_hr to 3_model_fitbit
</commit_message>
<xml_diff>
--- a/data/4_output/df_result (2019-08-12 1400 logreg).xlsx
+++ b/data/4_output/df_result (2019-08-12 1400 logreg).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cheekeet\OneDrive\Work\GA DSI\Lab\working-directory\project-capstone\data\4_output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{F89EC09F-BE4E-4FB0-BD74-1F25B0BF5A52}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{77A7F2A9-FA19-4F48-A50F-D0308158928B}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{F89EC09F-BE4E-4FB0-BD74-1F25B0BF5A52}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{0920D888-E460-4E63-99CB-9E1B8441CC96}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>y_test</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>rmse</t>
+  </si>
+  <si>
+    <t>df_activity</t>
   </si>
 </sst>
 </file>
@@ -593,21 +596,21 @@
   <dxfs count="2">
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -924,10 +927,13 @@
   <dimension ref="A1:F112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -940,10 +946,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1">
-        <v>0.70656370656370604</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -957,10 +960,10 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2">
-        <v>0.45045045045045001</v>
+        <v>0.70656370656370604</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -974,10 +977,10 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F3">
-        <v>10.4747659029078</v>
+        <v>0.45045045045045001</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -989,6 +992,12 @@
       </c>
       <c r="C4" t="b">
         <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>10.4747659029078</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2180,15 +2189,15 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D112">
-    <sortCondition ref="A2:A112"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D113">
+    <sortCondition ref="A3:A113"/>
   </sortState>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>TRUE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>